<commit_message>
Issue #3 has been resolved.
</commit_message>
<xml_diff>
--- a/PCB/SRv2.0/Documents/SR2_Power_Consumption.xlsx
+++ b/PCB/SRv2.0/Documents/SR2_Power_Consumption.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -46,6 +46,45 @@
     <t>PL_DDR4_VTT (0.6V)</t>
   </si>
   <si>
+    <t>AVDDL (1.2V)</t>
+  </si>
+  <si>
+    <t>AVDDH (2.5V)</t>
+  </si>
+  <si>
+    <t>DVDDL (1.2V)</t>
+  </si>
+  <si>
+    <t>VDDLS (1.2V)</t>
+  </si>
+  <si>
+    <t>VDDHS (2.5V)</t>
+  </si>
+  <si>
+    <t>VDDIO (2.5V)</t>
+  </si>
+  <si>
+    <t>VIO (1.8V)*</t>
+  </si>
+  <si>
+    <t>VBAT (3.7V)</t>
+  </si>
+  <si>
+    <t>VDDA2P5 (2.5V)</t>
+  </si>
+  <si>
+    <t>VDDA1P8 (1.8V)</t>
+  </si>
+  <si>
+    <t>VDDA1P0 (1.0V)</t>
+  </si>
+  <si>
+    <t>VDDIO (1.8V-3.3V)</t>
+  </si>
+  <si>
+    <t>USB 5.0V</t>
+  </si>
+  <si>
     <t>QSPI - MT25QU256ABA1EW7-0SIT</t>
   </si>
   <si>
@@ -59,6 +98,21 @@
   </si>
   <si>
     <t>PL SODIMM - 16GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMMC </t>
+  </si>
+  <si>
+    <t>ETH-Switch</t>
+  </si>
+  <si>
+    <t>WLAN, Bluetooth</t>
+  </si>
+  <si>
+    <t>ETH-Phy</t>
+  </si>
+  <si>
+    <t>USB 3.0 Power</t>
   </si>
 </sst>
 </file>
@@ -204,13 +258,52 @@
       <c r="K3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3">
         <v>1.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>2.0</v>
@@ -240,13 +333,52 @@
       <c r="K4" s="3">
         <v>0.0</v>
       </c>
+      <c r="L4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3">
         <v>2.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>1.0</v>
@@ -276,13 +408,52 @@
       <c r="K5" s="3">
         <v>0.0</v>
       </c>
+      <c r="L5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
         <v>3.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>1.0</v>
@@ -313,13 +484,52 @@
       <c r="K6" s="3">
         <v>0.0</v>
       </c>
+      <c r="L6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3">
         <v>4.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>1.0</v>
@@ -352,16 +562,58 @@
       <c r="K7" s="3">
         <v>0.0</v>
       </c>
+      <c r="L7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
         <v>5.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.0</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -387,6 +639,417 @@
       <c r="K8" s="5">
         <f>C8*500</f>
         <v>500</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E9">
+        <f>C9*80</f>
+        <v>320</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>460.0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>330.0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>750.0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R11" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="S11">
+        <f>3000/3.7</f>
+        <v>810.8108108</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T12" s="3">
+        <v>137.0</v>
+      </c>
+      <c r="U12" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="V12" s="3">
+        <v>108.0</v>
+      </c>
+      <c r="W12" s="3">
+        <v>24.0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>1000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>